<commit_message>
organize code for better use and read
</commit_message>
<xml_diff>
--- a/yallkora/SavingScrapingFiles/matchResults2.xlsx
+++ b/yallkora/SavingScrapingFiles/matchResults2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>Match Board</t>
   </si>
@@ -25,145 +25,76 @@
     <t>TV Channel</t>
   </si>
   <si>
-    <t>تشيلسي  4 : 0  ايفرتون</t>
-  </si>
-  <si>
-    <t>14:00</t>
+    <t>إنبي  0 : 1  بيراميدز</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>Ontime sports 1</t>
+  </si>
+  <si>
+    <t>طنطا‏  0 : 0  وادي دجلة</t>
+  </si>
+  <si>
+    <t>19:30</t>
+  </si>
+  <si>
+    <t>الأهلي  1 : 1  سموحة</t>
+  </si>
+  <si>
+    <t>ليفربول  2 : 3  اتلتيكو مدريد</t>
+  </si>
+  <si>
+    <t>22:00</t>
   </si>
   <si>
     <t>بى أن سبورت 2 HD</t>
   </si>
   <si>
-    <t>مانشستر يونايتد  2 : 0  مانشستر سيتي</t>
-  </si>
-  <si>
-    <t>16:30</t>
-  </si>
-  <si>
-    <t>أوساسونا  1 : 0  اسبانيول</t>
-  </si>
-  <si>
-    <t>13:00</t>
-  </si>
-  <si>
-    <t>بى أن سبورت 3 HD</t>
-  </si>
-  <si>
-    <t>بلد الوليد  1 : 4  اتليتك بلباو</t>
-  </si>
-  <si>
-    <t>15:00</t>
-  </si>
-  <si>
-    <t>ليفانتي  1 : 1  غرناطه</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>فياريال  1 : 2  ديبورتيفو ليجانيس</t>
-  </si>
-  <si>
-    <t>19:30</t>
-  </si>
-  <si>
-    <t>ريال بيتيس  2 : 1  ريال مدريد</t>
-  </si>
-  <si>
-    <t>22:00</t>
-  </si>
-  <si>
-    <t>بيراميدز  0 : 1  زاناكو</t>
+    <t>ب. س. جيرمان  2 : 0  بروسيا دورتموند</t>
   </si>
   <si>
     <t>بى أن سبورت 1HD</t>
   </si>
   <si>
-    <t>حسنية اغادير  2 : 0  النصر</t>
-  </si>
-  <si>
-    <t>18:00</t>
-  </si>
-  <si>
-    <t>حوريا كوناكري  2 : 0  أنيمبــــا</t>
-  </si>
-  <si>
-    <t>بى أن سبورت 7 HD</t>
-  </si>
-  <si>
-    <t>نهضة بركان  1 : 0  المصري</t>
-  </si>
-  <si>
-    <t>21:00</t>
-  </si>
-  <si>
-    <t>بارما  0 : 1  سبال</t>
-  </si>
-  <si>
-    <t>13:30</t>
-  </si>
-  <si>
-    <t>بى أن سبورت 4 HD</t>
-  </si>
-  <si>
-    <t>ميلان  1 : 2  جنوى</t>
-  </si>
-  <si>
-    <t>16:00</t>
-  </si>
-  <si>
-    <t>سامبدوريا  2 : 1  هيلاس فيرونا</t>
-  </si>
-  <si>
-    <t>أودينيزي  0 : 0  فيورنتينا</t>
-  </si>
-  <si>
-    <t>19:00</t>
-  </si>
-  <si>
-    <t>يوفنتوس  2 : 0  انترناسيونالي</t>
-  </si>
-  <si>
-    <t>21:45</t>
-  </si>
-  <si>
-    <t>بايرن ميونيخ  2 : 0  أوجسبورج</t>
+    <t>مونشنجلادباخ  2 : 1  كولن</t>
   </si>
   <si>
     <t>بى أن سبورت 5 HD</t>
   </si>
   <si>
-    <t>ماينز  1 : 1  ف.دوسلدورف</t>
-  </si>
-  <si>
-    <t>سانت اتيان  1 : 1  بوردو</t>
-  </si>
-  <si>
-    <t>بى أن سبورت 6 HD</t>
-  </si>
-  <si>
-    <t>رين  5 : 0  مونبيليه</t>
-  </si>
-  <si>
-    <t>ليل  1 : 0  ليون</t>
-  </si>
-  <si>
-    <t>موريرنسي  2 : 0  ماريتيمو</t>
-  </si>
-  <si>
-    <t>بيلينينسيش  0 : 0  فاماليكاو</t>
-  </si>
-  <si>
-    <t>جل فيسنتي  1 : 1  سانتا كلارا</t>
-  </si>
-  <si>
-    <t>سبورتينج لشبونة  2 : 0  ديسبورتيفو أفيس</t>
-  </si>
-  <si>
-    <t>باكوس فيريرا  1 : 2  فيتوريا جيماريش</t>
-  </si>
-  <si>
-    <t>أوليمبيك خريبكه  1 : 0  الدفاع الجديدي</t>
+    <t>ضمك  1 : 1  الهلال</t>
+  </si>
+  <si>
+    <t>15:10</t>
+  </si>
+  <si>
+    <t>الأتفـــــاق  1 : 0  الشباب</t>
+  </si>
+  <si>
+    <t>17:25</t>
+  </si>
+  <si>
+    <t>الفيحاء  0 : 2  أبها</t>
+  </si>
+  <si>
+    <t>17:45</t>
+  </si>
+  <si>
+    <t>التعاون  1 : 0  أهلي جدة</t>
+  </si>
+  <si>
+    <t>17:50</t>
+  </si>
+  <si>
+    <t>الاتحاد  1 : 2  الوحدة</t>
+  </si>
+  <si>
+    <t>19:45</t>
+  </si>
+  <si>
+    <t>النصر  4 : 1  الرائد</t>
   </si>
 </sst>
 </file>
@@ -523,14 +454,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
   </cols>
@@ -582,10 +514,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -593,13 +525,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,13 +539,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -621,13 +553,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -635,13 +567,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -649,13 +578,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
         <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,13 +589,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,13 +600,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -691,13 +611,10 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -705,205 +622,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>43</v>
-      </c>
-      <c r="C22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>46</v>
-      </c>
-      <c r="C25" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
         <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>